<commit_message>
creating a authentication table and frontend
</commit_message>
<xml_diff>
--- a/Documentasi/SchemanDatabase.xlsx
+++ b/Documentasi/SchemanDatabase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="8280"/>
+    <workbookView windowWidth="10668" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>Table</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>user_roles</t>
+  </si>
+  <si>
+    <t>role_id</t>
   </si>
   <si>
     <t>user_id</t>
@@ -773,23 +779,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -800,7 +800,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1325,10 +1325,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16" customHeight="1" outlineLevelCol="3"/>
@@ -1340,26 +1340,26 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -1437,12 +1437,12 @@
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:3">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
@@ -1453,35 +1453,35 @@
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:2">
-      <c r="A15" t="s">
+    <row r="15" customHeight="1" spans="1:1">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:1">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="16" customHeight="1" spans="1:3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:2">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" customHeight="1" spans="1:3">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
       <c r="B17" t="s">
         <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:2">
@@ -1489,76 +1489,76 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" customHeight="1" spans="1:2">
-      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:1">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:2">
+    </row>
+    <row r="20" customHeight="1" spans="1:3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:2">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="24" customHeight="1" spans="1:1">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" customHeight="1" spans="1:3">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:1">
-      <c r="A27" s="5" t="s">
-        <v>28</v>
+      <c r="A27" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:3">
@@ -1574,257 +1574,281 @@
     </row>
     <row r="29" customHeight="1" spans="1:2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="1:2">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" customHeight="1" spans="1:2">
+    <row r="30" customHeight="1" spans="1:1">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:2">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customHeight="1" spans="1:2">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:2">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="34" customHeight="1" spans="1:1">
-      <c r="A34" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" customHeight="1" spans="1:3">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" customHeight="1" spans="1:2">
-      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" customHeight="1" spans="1:1">
+      <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" customHeight="1" spans="1:1">
-      <c r="A38" s="5" t="s">
+    </row>
+    <row r="38" customHeight="1" spans="1:3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customHeight="1" spans="1:2">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" customHeight="1" spans="1:3">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:1">
+      <c r="A41" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:3">
+      <c r="A42" t="s">
         <v>5</v>
       </c>
-      <c r="B39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="1:2">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" customHeight="1" spans="1:2">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" customHeight="1" spans="1:1">
-      <c r="A42" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="1:3">
+    <row r="43" customHeight="1" spans="1:2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="44" customHeight="1" spans="1:2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" customHeight="1" spans="1:2">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" customHeight="1" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customHeight="1" spans="1:1">
+      <c r="A45" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" customHeight="1" spans="1:3">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:2">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" customHeight="1" spans="1:2">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" customHeight="1" spans="1:2">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="49" customHeight="1" spans="1:1">
-      <c r="A49" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" customHeight="1" spans="1:3">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:2">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" customHeight="1" spans="1:2">
-      <c r="A52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" customHeight="1" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" customHeight="1" spans="1:1">
+      <c r="A52" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" customHeight="1" spans="1:3">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="1:2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" customHeight="1" spans="1:2">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" customHeight="1" spans="1:2">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="55" customHeight="1" spans="1:1">
-      <c r="A55" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" customHeight="1" spans="1:3">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="57" customHeight="1" spans="1:2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" customHeight="1" spans="1:2">
-      <c r="A58" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" customHeight="1" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" customHeight="1" spans="1:1">
+      <c r="A58" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" customHeight="1" spans="1:3">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" customHeight="1" spans="1:2">
       <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" customHeight="1" spans="1:2">
+      <c r="A61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" customHeight="1" spans="1:2">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" customHeight="1" spans="1:2">
+      <c r="A63" t="s">
         <v>19</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>